<commit_message>
Modified the dummy_class data to have a column of numbers as strings
</commit_message>
<xml_diff>
--- a/pandas-data/dummy_class.xlsx
+++ b/pandas-data/dummy_class.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/theChest/my-github/data/pandas-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FC4C51C5-0054-A745-B58D-C0E736D0130A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{4072E354-4675-4142-A89F-7715EC8FBBBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18440" yWindow="500" windowWidth="32760" windowHeight="31500"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="78">
   <si>
     <t>Name</t>
   </si>
@@ -175,6 +177,96 @@
   </si>
   <si>
     <t>This is a dummy set of class data created to show how to use dataframes.</t>
+  </si>
+  <si>
+    <t>18.960</t>
+  </si>
+  <si>
+    <t>17.440</t>
+  </si>
+  <si>
+    <t>15.560</t>
+  </si>
+  <si>
+    <t>16.360</t>
+  </si>
+  <si>
+    <t>17.896</t>
+  </si>
+  <si>
+    <t>14.088</t>
+  </si>
+  <si>
+    <t>16.720</t>
+  </si>
+  <si>
+    <t>16.400</t>
+  </si>
+  <si>
+    <t>13.680</t>
+  </si>
+  <si>
+    <t>9.040</t>
+  </si>
+  <si>
+    <t>16.880</t>
+  </si>
+  <si>
+    <t>17.000</t>
+  </si>
+  <si>
+    <t>16.680</t>
+  </si>
+  <si>
+    <t>14.128</t>
+  </si>
+  <si>
+    <t>15.720</t>
+  </si>
+  <si>
+    <t>14.680</t>
+  </si>
+  <si>
+    <t>17.648</t>
+  </si>
+  <si>
+    <t>15.000</t>
+  </si>
+  <si>
+    <t>16.016</t>
+  </si>
+  <si>
+    <t>15.480</t>
+  </si>
+  <si>
+    <t>14.360</t>
+  </si>
+  <si>
+    <t>18.080</t>
+  </si>
+  <si>
+    <t>15.920</t>
+  </si>
+  <si>
+    <t>18.440</t>
+  </si>
+  <si>
+    <t>11.000</t>
+  </si>
+  <si>
+    <t>16.800</t>
+  </si>
+  <si>
+    <t>17.760</t>
+  </si>
+  <si>
+    <t>10.280</t>
+  </si>
+  <si>
+    <t>15.040</t>
+  </si>
+  <si>
+    <t>13.816</t>
   </si>
 </sst>
 </file>
@@ -580,7 +672,7 @@
   <dimension ref="A1:G37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="K53" sqref="K53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -633,8 +725,8 @@
       <c r="E3" s="2">
         <v>20.204999999999998</v>
       </c>
-      <c r="F3" s="2">
-        <v>18.96</v>
+      <c r="F3" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G3" s="2">
         <v>21.25</v>
@@ -656,8 +748,8 @@
       <c r="E4" s="2">
         <v>13.47</v>
       </c>
-      <c r="F4" s="2">
-        <v>17.440000000000001</v>
+      <c r="F4" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="G4" s="2">
         <v>18.75</v>
@@ -679,8 +771,8 @@
       <c r="E5" s="2">
         <v>18.366</v>
       </c>
-      <c r="F5" s="2">
-        <v>15.560000000000002</v>
+      <c r="F5" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G5" s="2">
         <v>43.75</v>
@@ -702,8 +794,8 @@
       <c r="E6" s="2">
         <v>18.366</v>
       </c>
-      <c r="F6" s="2">
-        <v>16.36</v>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="G6" s="2">
         <v>18.75</v>
@@ -725,8 +817,8 @@
       <c r="E7" s="2">
         <v>15.305999999999999</v>
       </c>
-      <c r="F7" s="2">
-        <v>17.896000000000001</v>
+      <c r="F7" s="2" t="s">
+        <v>52</v>
       </c>
       <c r="G7" s="2">
         <v>17.5</v>
@@ -748,8 +840,8 @@
       <c r="E8" s="2">
         <v>12.246</v>
       </c>
-      <c r="F8" s="2">
-        <v>14.088000000000001</v>
+      <c r="F8" s="2" t="s">
+        <v>53</v>
       </c>
       <c r="G8" s="2">
         <v>32.5</v>
@@ -771,8 +863,8 @@
       <c r="E9" s="2">
         <v>16.53</v>
       </c>
-      <c r="F9" s="2">
-        <v>16.72</v>
+      <c r="F9" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="G9" s="2">
         <v>31.25</v>
@@ -794,8 +886,8 @@
       <c r="E10" s="2">
         <v>18.981000000000002</v>
       </c>
-      <c r="F10" s="2">
-        <v>16.399999999999999</v>
+      <c r="F10" s="2" t="s">
+        <v>55</v>
       </c>
       <c r="G10" s="2">
         <v>43.75</v>
@@ -817,8 +909,8 @@
       <c r="E11" s="2">
         <v>15.305999999999999</v>
       </c>
-      <c r="F11" s="2">
-        <v>13.680000000000001</v>
+      <c r="F11" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="G11" s="2">
         <v>47.5</v>
@@ -840,8 +932,8 @@
       <c r="E12" s="2">
         <v>17.754000000000001</v>
       </c>
-      <c r="F12" s="2">
-        <v>9.0400000000000009</v>
+      <c r="F12" s="2" t="s">
+        <v>57</v>
       </c>
       <c r="G12" s="2">
         <v>41.25</v>
@@ -863,8 +955,8 @@
       <c r="E13" s="2">
         <v>19.593</v>
       </c>
-      <c r="F13" s="2">
-        <v>16.880000000000003</v>
+      <c r="F13" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="G13" s="2">
         <v>32.5</v>
@@ -886,8 +978,8 @@
       <c r="E14" s="2">
         <v>26.328000000000003</v>
       </c>
-      <c r="F14" s="2">
-        <v>17</v>
+      <c r="F14" s="2" t="s">
+        <v>59</v>
       </c>
       <c r="G14" s="2">
         <v>50</v>
@@ -909,8 +1001,8 @@
       <c r="E15" s="2">
         <v>14.081999999999999</v>
       </c>
-      <c r="F15" s="2">
-        <v>16.68</v>
+      <c r="F15" s="2" t="s">
+        <v>60</v>
       </c>
       <c r="G15" s="2">
         <v>41.25</v>
@@ -932,8 +1024,8 @@
       <c r="E16" s="2">
         <v>22.041</v>
       </c>
-      <c r="F16" s="2">
-        <v>14.128</v>
+      <c r="F16" s="2" t="s">
+        <v>61</v>
       </c>
       <c r="G16" s="2">
         <v>25</v>
@@ -953,8 +1045,8 @@
         <v>46</v>
       </c>
       <c r="E17" s="2"/>
-      <c r="F17" s="2">
-        <v>15.72</v>
+      <c r="F17" s="2" t="s">
+        <v>62</v>
       </c>
       <c r="G17" s="2">
         <v>35</v>
@@ -976,8 +1068,8 @@
       <c r="E18" s="2">
         <v>20.817</v>
       </c>
-      <c r="F18" s="2">
-        <v>14.680000000000001</v>
+      <c r="F18" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G18" s="2">
         <v>20</v>
@@ -999,8 +1091,8 @@
       <c r="E19" s="2">
         <v>22.653000000000002</v>
       </c>
-      <c r="F19" s="2">
-        <v>17.648000000000003</v>
+      <c r="F19" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G19" s="2">
         <v>50</v>
@@ -1022,8 +1114,8 @@
       <c r="E20" s="2">
         <v>19.593</v>
       </c>
-      <c r="F20" s="2">
-        <v>14.680000000000001</v>
+      <c r="F20" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="G20" s="2"/>
     </row>
@@ -1043,8 +1135,8 @@
       <c r="E21" s="2">
         <v>18.981000000000002</v>
       </c>
-      <c r="F21" s="2">
-        <v>15</v>
+      <c r="F21" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="G21" s="2">
         <v>33.75</v>
@@ -1066,8 +1158,8 @@
       <c r="E22" s="2">
         <v>15.305999999999999</v>
       </c>
-      <c r="F22" s="2">
-        <v>16.015999999999998</v>
+      <c r="F22" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="G22" s="2">
         <v>43.75</v>
@@ -1089,8 +1181,8 @@
       <c r="E23" s="2">
         <v>12.857999999999999</v>
       </c>
-      <c r="F23" s="2">
-        <v>15.48</v>
+      <c r="F23" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="2">
         <v>46.25</v>
@@ -1112,8 +1204,8 @@
       <c r="E24" s="2">
         <v>23.877000000000002</v>
       </c>
-      <c r="F24" s="2">
-        <v>17.648000000000003</v>
+      <c r="F24" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="G24" s="2">
         <v>32.5</v>
@@ -1135,8 +1227,8 @@
       <c r="E25" s="2">
         <v>15.918000000000003</v>
       </c>
-      <c r="F25" s="2">
-        <v>14.360000000000001</v>
+      <c r="F25" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G25" s="2">
         <v>41.25</v>
@@ -1158,8 +1250,8 @@
       <c r="E26" s="2">
         <v>22.041</v>
       </c>
-      <c r="F26" s="2">
-        <v>16.880000000000003</v>
+      <c r="F26" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="G26" s="2">
         <v>22.5</v>
@@ -1181,8 +1273,8 @@
       <c r="E27" s="2">
         <v>19.593</v>
       </c>
-      <c r="F27" s="2">
-        <v>14.360000000000001</v>
+      <c r="F27" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G27" s="2">
         <v>30</v>
@@ -1204,8 +1296,8 @@
       <c r="E28" s="2">
         <v>12.857999999999999</v>
       </c>
-      <c r="F28" s="2">
-        <v>18.080000000000002</v>
+      <c r="F28" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="G28" s="2">
         <v>47.5</v>
@@ -1227,8 +1319,8 @@
       <c r="E29" s="2">
         <v>23.265000000000001</v>
       </c>
-      <c r="F29" s="2">
-        <v>14.360000000000001</v>
+      <c r="F29" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="G29" s="2">
         <v>31.25</v>
@@ -1250,8 +1342,8 @@
       <c r="E30" s="2">
         <v>20.817</v>
       </c>
-      <c r="F30" s="2">
-        <v>15.919999999999998</v>
+      <c r="F30" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="G30" s="2">
         <v>16.25</v>
@@ -1271,8 +1363,8 @@
         <v>45</v>
       </c>
       <c r="E31" s="2"/>
-      <c r="F31" s="2">
-        <v>18.440000000000001</v>
+      <c r="F31" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="G31" s="2">
         <v>38.75</v>
@@ -1294,8 +1386,8 @@
       <c r="E32" s="2">
         <v>18.366</v>
       </c>
-      <c r="F32" s="2">
-        <v>11</v>
+      <c r="F32" s="2" t="s">
+        <v>72</v>
       </c>
       <c r="G32" s="2">
         <v>28.749999999999996</v>
@@ -1317,8 +1409,8 @@
       <c r="E33" s="2">
         <v>18.366</v>
       </c>
-      <c r="F33" s="2">
-        <v>16.8</v>
+      <c r="F33" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="G33" s="2">
         <v>36.25</v>
@@ -1340,8 +1432,8 @@
       <c r="E34" s="2">
         <v>22.653000000000002</v>
       </c>
-      <c r="F34" s="2">
-        <v>17.760000000000002</v>
+      <c r="F34" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="G34" s="2">
         <v>16.25</v>
@@ -1363,8 +1455,8 @@
       <c r="E35" s="2">
         <v>16.53</v>
       </c>
-      <c r="F35" s="2">
-        <v>10.28</v>
+      <c r="F35" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="G35" s="2"/>
     </row>
@@ -1384,8 +1476,8 @@
       <c r="E36" s="2">
         <v>17.754000000000001</v>
       </c>
-      <c r="F36" s="2">
-        <v>15.04</v>
+      <c r="F36" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="G36" s="2">
         <v>25</v>
@@ -1407,8 +1499,8 @@
       <c r="E37" s="2">
         <v>20.817</v>
       </c>
-      <c r="F37" s="2">
-        <v>13.815999999999999</v>
+      <c r="F37" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="G37" s="2"/>
     </row>

</xml_diff>